<commit_message>
add new exercises, update anki deck/wordlist, ref patterns
- updated anki deck/wordlist for Lesson 13 vocab. (3rd ed.)
- updated kanji reference pattern for 肉.
- added the following exercises.

# Lesson 13 (3rd ed.)
- Kanji Practice: Stroke Order
- Kanji Vocabulary: 物, 鳥, and 料
- Kanji Vocabulary: 理, 特, and 安
- Kanji Vocabulary: 販, 肉, and 悪
- Kanji Vocabulary: 体, 同, 着, and 空
- Kanji Vocabulary: 港, 昼, and 海
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-13.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-13.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1357,6 +1357,834 @@
         </is>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>食べ物|たべもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>drink</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>飲み物|のみもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>things</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>物|もの</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>shopping</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>買い物|かいもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>animal</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>動物|どうぶつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>commodity prices</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>物価|ぶっか</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>bird</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>鳥|とり</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>grilled chicken</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>焼き鳥|やきとり</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>swan</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>白鳥|はくちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>cooking</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>料理|りょうり</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>charge</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>料金|りょうきん</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>tuition</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>授業料|じゅぎょうりょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>salary</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>給料|きゅうりょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>cooking</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>料理|りょうり</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>理由|りゆう</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>geography</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>地理|ちり</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>impossible</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>無理な|むりな</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>especially</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>特に|とくに</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>特別な|とくべつな</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>characteristic</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>特徴|とくちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>super express</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>特急|とっきゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>cheap</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>安い|やすい</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>safe</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>安全な|あんぜんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>relief</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>安心|あんしん</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>anxious; worried</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>不安な|ふあんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>rice; meal</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>ご飯|ごはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>breakfast</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>朝ご飯|あさごはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>lunch</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>昼ご飯|ひるごはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>晩ご飯|ばんごはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>meat</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>肉|にく</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>beef</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>牛肉|ぎゅうにく</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>pork</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>豚肉|ぶたにく</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>meat shop</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>肉屋|にくや</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>muscle</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>筋肉|きんにく</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>bad</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>悪い|わるい</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>to feel sick</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>気分が悪い|きぶんがわるい</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>the worst</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>最悪|さいあく</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>devil</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>悪魔|あくま</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>body</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>体|からだ</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>body weight</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>体重|たいじゅう</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>gymnastics; physical exercises</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>体操|たいそう</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>the same</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>同じ|おなじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>coworker</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>同僚|どうりょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>classmate</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>同級生|どうきゅうせい</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>same time</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>同時|どうじ</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>to arrive</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>着く|つく</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>to wear</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>着る|きる</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>kimono</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>着物|きもの</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>swimwear</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>水着|みずぎ</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>arriving at Osaka</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>大阪着|おおさかちゃく</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>airport</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>空港|くうこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>air</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>空気|くうき</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>sky</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>空|そら</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>to be vacant</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>空く|あく</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>karate</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>空手|からて</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>airport</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>空港|くうこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Kobe Port</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>神戸港|こうべこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>port</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>港|みなと</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Hong Kong</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>香港|ほんこん</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>noon; daytime</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>昼|ひる</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>lunch</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>昼ご飯|ひるごはん</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>nap</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>昼寝|ひるね</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>lunch break</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>昼休み|ひるやすみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>lunch (formal)</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>昼食|ちゅうしょく</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>sea</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>海|うみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>the Japan Sea</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>日本海|にほんかい</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>overseas</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>海外|かいがい</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>coast</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>海岸|かいがん</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Hokkaido</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>北海道|ほっかいどう</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>